<commit_message>
Add visualization of metrices
</commit_message>
<xml_diff>
--- a/food_items.xlsx
+++ b/food_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Python programs\HealthTeracker App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBBEF00-3D2E-430F-828E-AEC6904BFED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2503BE4B-9925-4BA0-9456-8FEBF643FD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Food Item</t>
   </si>
@@ -145,13 +145,31 @@
   </si>
   <si>
     <t>calories</t>
+  </si>
+  <si>
+    <t>Fish (Bombil, Cooked)</t>
+  </si>
+  <si>
+    <t>101 g cooked</t>
+  </si>
+  <si>
+    <t>1 scoop/serving(39g)</t>
+  </si>
+  <si>
+    <t>Protein Shake (Fuel one whey)</t>
+  </si>
+  <si>
+    <t>Rice(cooked)</t>
+  </si>
+  <si>
+    <t>Toor dal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +181,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -216,24 +240,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -526,436 +570,535 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>18</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>20</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>265</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>0.2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>116</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>0.8</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>127</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>2.7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>164</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>52</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>0.5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>345</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>2.5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>0.2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>128</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>3.5</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>168</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>3.5</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>158</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>3</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>192</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>6</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>8</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>250</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>200</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>3.5</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>4</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>61</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="3">
+        <v>165</v>
+      </c>
+      <c r="F14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3">
+        <v>60.7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <v>287</v>
+      </c>
+      <c r="F15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>115</v>
+      </c>
+      <c r="F16" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3">
+        <v>134</v>
+      </c>
+      <c r="F17" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>165</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="C18" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>155</v>
+      </c>
+      <c r="F18" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3">
+        <v>26</v>
+      </c>
+      <c r="D19" s="3">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3">
+        <v>294</v>
+      </c>
+      <c r="F19" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>99</v>
+      </c>
+      <c r="F20" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3">
+        <v>15</v>
+      </c>
+      <c r="E21" s="3">
+        <v>262</v>
+      </c>
+      <c r="F21" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3">
+        <v>290</v>
+      </c>
+      <c r="F22" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3">
+        <v>20</v>
+      </c>
+      <c r="E23" s="3">
+        <v>550</v>
+      </c>
+      <c r="F23" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="3">
+        <v>24</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2.11</v>
+      </c>
+      <c r="E24" s="3">
+        <v>150</v>
+      </c>
+      <c r="F24" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E25" s="6">
+        <v>130</v>
+      </c>
+      <c r="F25" s="7">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="5">
+        <v>107</v>
+      </c>
+      <c r="F26" s="5">
         <v>23</v>
       </c>
-      <c r="C15" s="2">
-        <v>17</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>134</v>
-      </c>
-      <c r="F15" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="2">
-        <v>13</v>
-      </c>
-      <c r="D16" s="2">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2">
-        <v>155</v>
-      </c>
-      <c r="F16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2">
-        <v>26</v>
-      </c>
-      <c r="D17" s="2">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2">
-        <v>294</v>
-      </c>
-      <c r="F17" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="2">
-        <v>24</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>99</v>
-      </c>
-      <c r="F18" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="2">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2">
-        <v>262</v>
-      </c>
-      <c r="F19" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="2">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2">
-        <v>14</v>
-      </c>
-      <c r="E20" s="2">
-        <v>290</v>
-      </c>
-      <c r="F20" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="2">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2">
-        <v>550</v>
-      </c>
-      <c r="F21" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>